<commit_message>
Modifiying the Power Plant formating  notebook
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigBE1.xlsx
+++ b/ConfigFiles/ConfigBE1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="249">
   <si>
     <t xml:space="preserve">Dispa-SET Configuration File (v20.02)</t>
   </si>
@@ -33,7 +33,7 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Belgium configuration file with 2015 data</t>
+    <t xml:space="preserve">Belgium configuration file with 2023 data</t>
   </si>
   <si>
     <t xml:space="preserve">Legend</t>
@@ -57,7 +57,7 @@
     <t xml:space="preserve">Relative Path</t>
   </si>
   <si>
-    <t xml:space="preserve">Simulations/simulationBE1</t>
+    <t xml:space="preserve">Simulations/simulationBE_No_Clustering_No_Reservoir_Level</t>
   </si>
   <si>
     <t xml:space="preserve">This section defines the output of the pre-processing (which is the input of the DispaSet solver)</t>
@@ -135,601 +135,598 @@
     <t xml:space="preserve">List</t>
   </si>
   <si>
+    <t xml:space="preserve">No clustering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This sections defines parameters that influence the formulation of the problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserve calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These parameters influence both the pre-processing (e.g. in LP clustering, all units are aggregated by type)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allow Curtailment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and the solver (some constraints are removed when solving in LP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro Scheduling Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro scheduling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These parameters influence how HDAM and HPHS units are operated (e.g. if Standard: scaled reservoir levels are computed internally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro scheduling horizon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These parameters influence the horizon of the hydro scheduling (e.g. if Annual: reservoirs are computed for the whole year, if Stop-date driven: computation of reservoirs is driven by the start and stop date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial/Final resevoir levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-&gt; Initial level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This value imposes the inital (relative) reservoir levels if the option is set to true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;- Final level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This value imposes the final (relative) reservoir levels if the option is set to true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/Load_RealTime/##/1h/2023.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flexible Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/OutageFactors/##/1h/2023.csv </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section provides the paths to the raw data used to generate the Dispa-SET simulation template. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power plant data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/PowerPlants/##/2023.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The path is an absolute path or a relative path to this config file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renewables AF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/AvailabilityFactors/##/1h/2023.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Shedding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For datasets which have one file per country, replace the country code (2 characters) in the path by ##. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/NTC/1h/2023.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for example: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical flows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/CrossBorderFlows/1h/2023.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../data/Demand/##/2014/load.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scaled inflows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/HydroData/ScaledInflows/##/1h/2023.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">will fetch one load.csv file per country, by replacing ## with FR, DE, NL, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reservoir Levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperatures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geo Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2 Demand (P2H2 - rigid)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2 Demand (P2Liquid - flexible)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2 Capacities (P2Liquid - flexible)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserves Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserves Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demand flexibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of equivalent storage hours for the flexibile demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of quick start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of the 2U reserve that can be covered by quick start units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: https://dev-rad-carbon-pricing.pantheonsite.io/about#download-data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Unserved Heat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Shedding Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The least amount that customers are willing to recieve to reduce the electricity demand. EUR/MWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Transmission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price related to the usage of tranmission lines (in €/MWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Unserved H2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curtailment Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Nuclear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Black coal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/FuelPrices/Coal/2015.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/FuelPrices/Gas/2015.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All fuel prices are in EUR/MWh of primary energy (lower heating value)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Fuel-Oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/FuelPrices/Oil/2015.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ahdb.org.uk/fuel-prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/FuelPrices/Biomass/2015.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Lignite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Peat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Ammonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of Lost Load (VOLL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of lost load  in EUR/MWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Spillage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost occurring due to involuntary water spillage in hydro resrvoirs EUR/MWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of water (for unsatisfied water reservoir levels) EUR/MWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Countries to consider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUTS1 codes (ISO 3166-1 standard) of the simulated countries.                                      NB: all the selected countries must be present in the data files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZZ3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NB: Ireland (IE) includes Northern Ireland. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NB: UK is not considered as zone but GB is.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input modifiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mult. Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The input modifies can be used to quickly modify the data from the database. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The specified factor scales up or down the capacity and the generation of the specified technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserve Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participation to reserve markets (CHP units)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participation to reserve markets (Non-CHP units)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2HT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HYHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WSHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REHE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALKE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WTOF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOXE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BATS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEVS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2GS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End of the Config file. This must be line number 325!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulation Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resrve calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacity Correction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display Warning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zonal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop-date driven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LP clustered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Probabilistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add plants</t>
+  </si>
+  <si>
     <t xml:space="preserve">Integer clustering</t>
   </si>
   <si>
-    <t xml:space="preserve">This sections defines parameters that influence the formulation of the problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reserve calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">These parameters influence both the pre-processing (e.g. in LP clustering, all units are aggregated by type)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allow Curtailment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">and the solver (some constraints are removed when solving in LP)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hydro Scheduling Options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hydro scheduling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">These parameters influence how HDAM and HPHS units are operated (e.g. if Standard: scaled reservoir levels are computed internally</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hydro scheduling horizon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">These parameters influence the horizon of the hydro scheduling (e.g. if Annual: reservoirs are computed for the whole year, if Stop-date driven: computation of reservoirs is driven by the start and stop date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial/Final resevoir levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-&gt; Initial level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This value imposes the inital (relative) reservoir levels if the option is set to true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;- Final level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This value imposes the final (relative) reservoir levels if the option is set to true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/Load_RealTime/##/1h/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flexible Demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/OutageFactors/##/1h/2023.csv </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This section provides the paths to the raw data used to generate the Dispa-SET simulation template. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power plant data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/PowerPlants/##/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The path is an absolute path or a relative path to this config file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renewables AF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/AvailabilityFactors/##/1h/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load Shedding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For datasets which have one file per country, replace the country code (2 characters) in the path by ##. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NTC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/NTC/1h/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">for example: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Historical flows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/CrossBorderFlows/1h/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../data/Demand/##/2014/load.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scaled inflows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/HydroData/ScaledInflows/##/1h/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">will fetch one load.csv file per country, by replacing ## with FR, DE, NL, etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reservoir Levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/HydroData/ReservoirLevel/##/1h/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heat Demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperatures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geo Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2 Demand (P2H2 - rigid)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2 Demand (P2Liquid - flexible)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2 Capacities (P2Liquid - flexible)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reserves Up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reserves Down</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demand flexibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of equivalent storage hours for the flexibile demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share of quick start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share of the 2U reserve that can be covered by quick start units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of CO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source: https://dev-rad-carbon-pricing.pantheonsite.io/about#download-data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Unserved Heat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load Shedding Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The least amount that customers are willing to recieve to reduce the electricity demand. EUR/MWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Transmission</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price related to the usage of tranmission lines (in €/MWh)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Unserved H2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Curtailment Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Nuclear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Black coal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/FuelPrices/Coal/2015.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/FuelPrices/Gas/2015.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All fuel prices are in EUR/MWh of primary energy (lower heating value)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Fuel-Oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/FuelPrices/Oil/2015.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://ahdb.org.uk/fuel-prices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/FuelPrices/Biomass/2015.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Lignite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Peat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Ammonia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value of Lost Load (VOLL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value of lost load  in EUR/MWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Spillage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost occurring due to involuntary water spillage in hydro resrvoirs EUR/MWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value of water (for unsatisfied water reservoir levels) EUR/MWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone Options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Active zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Countries to consider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUTS1 codes (ISO 3166-1 standard) of the simulated countries.                                      NB: all the selected countries must be present in the data files</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZZ3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NB: Ireland (IE) includes Northern Ireland. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NB: UK is not considered as zone but GB is.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input modifiers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mult. Factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The input modifies can be used to quickly modify the data from the database. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The specified factor scales up or down the capacity and the generation of the specified technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reserve Options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participation to reserve markets (CHP units)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participation to reserve markets (Non-CHP units)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2HT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HROR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HPHS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HYHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WSHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHOT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REHE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALKE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WTOF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WTON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOXE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BATS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DMFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BEVS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2GS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCSP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End of the Config file. This must be line number 325!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simulation Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resrve calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacity Correction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ignore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Display Warning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zonal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stop-date driven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LP clustered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Probabilistic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add plants</t>
-  </si>
-  <si>
     <t xml:space="preserve">Exogenous</t>
   </si>
   <si>
     <t xml:space="preserve">Scale-up capacities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No clustering</t>
   </si>
   <si>
     <t xml:space="preserve">BIO</t>
@@ -956,7 +953,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1143,6 +1140,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1336,8 +1337,8 @@
   </sheetPr>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K38" activeCellId="0" sqref="K38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C134" activeCellId="0" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2074,16 +2075,14 @@
       <c r="B134" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C134" s="32" t="s">
-        <v>81</v>
-      </c>
+      <c r="C134" s="32"/>
       <c r="D134" s="25" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B135" s="19" t="s">
         <v>10</v>
@@ -2095,7 +2094,7 @@
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B136" s="19" t="s">
         <v>10</v>
@@ -2108,7 +2107,7 @@
     </row>
     <row r="137" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B137" s="19" t="s">
         <v>10</v>
@@ -2120,7 +2119,7 @@
     </row>
     <row r="138" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B138" s="19" t="s">
         <v>10</v>
@@ -2129,7 +2128,7 @@
     </row>
     <row r="139" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B139" s="19" t="s">
         <v>10</v>
@@ -2138,7 +2137,7 @@
     </row>
     <row r="140" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B140" s="19" t="s">
         <v>10</v>
@@ -2167,7 +2166,7 @@
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="161" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B161" s="19" t="s">
         <v>10</v>
@@ -2176,7 +2175,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B162" s="19" t="s">
         <v>10</v>
@@ -2185,7 +2184,7 @@
     </row>
     <row r="163" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E163" s="21" t="s">
         <v>53</v>
@@ -2194,12 +2193,12 @@
         <v>4</v>
       </c>
       <c r="H163" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E164" s="21" t="s">
         <v>53</v>
@@ -2208,13 +2207,13 @@
         <v>0.5</v>
       </c>
       <c r="H164" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="166" s="18" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B166" s="16"/>
       <c r="C166" s="17"/>
@@ -2226,7 +2225,7 @@
     </row>
     <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B167" s="19" t="s">
         <v>10</v>
@@ -2242,12 +2241,12 @@
         <v>88.55</v>
       </c>
       <c r="H167" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B168" s="19" t="s">
         <v>10</v>
@@ -2265,7 +2264,7 @@
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B169" s="19" t="s">
         <v>10</v>
@@ -2281,12 +2280,12 @@
         <v>1500</v>
       </c>
       <c r="H169" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B170" s="19" t="s">
         <v>10</v>
@@ -2302,12 +2301,12 @@
         <v>0</v>
       </c>
       <c r="H170" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B171" s="19" t="s">
         <v>10</v>
@@ -2325,7 +2324,7 @@
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B172" s="19" t="s">
         <v>10</v>
@@ -2351,7 +2350,7 @@
     <row r="180" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="181" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B181" s="19" t="s">
         <v>10</v>
@@ -2367,13 +2366,13 @@
     </row>
     <row r="182" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B182" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C182" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D182" s="25" t="s">
         <v>20</v>
@@ -2387,13 +2386,13 @@
     </row>
     <row r="183" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B183" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C183" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D183" s="25" t="s">
         <v>20</v>
@@ -2405,18 +2404,18 @@
         <v>44</v>
       </c>
       <c r="H183" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B184" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C184" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D184" s="25" t="s">
         <v>20</v>
@@ -2428,18 +2427,18 @@
         <v>61</v>
       </c>
       <c r="H184" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B185" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C185" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D185" s="25" t="s">
         <v>20</v>
@@ -2453,7 +2452,7 @@
     </row>
     <row r="186" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B186" s="19" t="s">
         <v>10</v>
@@ -2471,7 +2470,7 @@
     </row>
     <row r="187" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B187" s="19" t="s">
         <v>10</v>
@@ -2489,7 +2488,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B188" s="19" t="s">
         <v>10</v>
@@ -2522,7 +2521,7 @@
     <row r="204" customFormat="false" ht="13.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="205" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E205" s="21" t="s">
         <v>53</v>
@@ -2531,12 +2530,12 @@
         <v>100000</v>
       </c>
       <c r="H205" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="206" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E206" s="21" t="s">
         <v>53</v>
@@ -2545,12 +2544,12 @@
         <v>401</v>
       </c>
       <c r="H206" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="207" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E207" s="21" t="s">
         <v>53</v>
@@ -2559,7 +2558,7 @@
         <v>400</v>
       </c>
       <c r="H207" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2583,45 +2582,45 @@
     </row>
     <row r="225" s="41" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B225" s="38" t="s">
         <v>14</v>
       </c>
       <c r="C225" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D225" s="39" t="s">
         <v>125</v>
-      </c>
-      <c r="D225" s="39" t="s">
-        <v>126</v>
       </c>
       <c r="E225" s="38" t="s">
         <v>14</v>
       </c>
       <c r="F225" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="G225" s="12" t="s">
         <v>125</v>
-      </c>
-      <c r="G225" s="12" t="s">
-        <v>126</v>
       </c>
       <c r="H225" s="40"/>
     </row>
     <row r="226" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B226" s="42" t="s">
         <v>127</v>
       </c>
-      <c r="B226" s="42" t="s">
+      <c r="C226" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D226" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E226" s="42" t="s">
         <v>128</v>
-      </c>
-      <c r="C226" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D226" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E226" s="42" t="s">
-        <v>129</v>
       </c>
       <c r="F226" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2634,21 +2633,21 @@
     </row>
     <row r="227" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="43" t="s">
+        <v>129</v>
+      </c>
+      <c r="B227" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="B227" s="42" t="s">
+      <c r="C227" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D227" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E227" s="42" t="s">
         <v>131</v>
-      </c>
-      <c r="C227" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D227" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E227" s="42" t="s">
-        <v>132</v>
       </c>
       <c r="F227" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2662,18 +2661,18 @@
     <row r="228" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="43"/>
       <c r="B228" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="C228" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D228" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E228" s="42" t="s">
         <v>133</v>
-      </c>
-      <c r="C228" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D228" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E228" s="42" t="s">
-        <v>134</v>
       </c>
       <c r="F228" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2687,18 +2686,18 @@
     <row r="229" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="43"/>
       <c r="B229" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="C229" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D229" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E229" s="42" t="s">
         <v>135</v>
-      </c>
-      <c r="C229" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D229" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E229" s="42" t="s">
-        <v>136</v>
       </c>
       <c r="F229" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2712,18 +2711,18 @@
     <row r="230" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="43"/>
       <c r="B230" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="C230" s="23" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D230" s="23" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E230" s="42" t="s">
         <v>137</v>
-      </c>
-      <c r="C230" s="23" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D230" s="23" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E230" s="42" t="s">
-        <v>138</v>
       </c>
       <c r="F230" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2737,18 +2736,18 @@
     <row r="231" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="43"/>
       <c r="B231" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="C231" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D231" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E231" s="42" t="s">
         <v>139</v>
-      </c>
-      <c r="C231" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D231" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E231" s="42" t="s">
-        <v>140</v>
       </c>
       <c r="F231" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2762,18 +2761,18 @@
     <row r="232" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="43"/>
       <c r="B232" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="C232" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D232" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E232" s="42" t="s">
         <v>141</v>
-      </c>
-      <c r="C232" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D232" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E232" s="42" t="s">
-        <v>142</v>
       </c>
       <c r="F232" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2787,18 +2786,18 @@
     <row r="233" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="43"/>
       <c r="B233" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="C233" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D233" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E233" s="42" t="s">
         <v>143</v>
-      </c>
-      <c r="C233" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D233" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E233" s="42" t="s">
-        <v>144</v>
       </c>
       <c r="F233" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2812,18 +2811,18 @@
     <row r="234" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="43"/>
       <c r="B234" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="C234" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D234" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E234" s="42" t="s">
         <v>145</v>
-      </c>
-      <c r="C234" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D234" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E234" s="42" t="s">
-        <v>146</v>
       </c>
       <c r="F234" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2837,18 +2836,18 @@
     <row r="235" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="43"/>
       <c r="B235" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="C235" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D235" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E235" s="42" t="s">
         <v>147</v>
-      </c>
-      <c r="C235" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D235" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E235" s="42" t="s">
-        <v>148</v>
       </c>
       <c r="F235" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2862,18 +2861,18 @@
     <row r="236" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="43"/>
       <c r="B236" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="C236" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D236" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E236" s="42" t="s">
         <v>149</v>
-      </c>
-      <c r="C236" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D236" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E236" s="42" t="s">
-        <v>150</v>
       </c>
       <c r="F236" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2887,18 +2886,18 @@
     <row r="237" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="43"/>
       <c r="B237" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="C237" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D237" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E237" s="42" t="s">
         <v>151</v>
-      </c>
-      <c r="C237" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D237" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E237" s="42" t="s">
-        <v>152</v>
       </c>
       <c r="F237" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2912,18 +2911,18 @@
     <row r="238" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="43"/>
       <c r="B238" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="C238" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D238" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E238" s="42" t="s">
         <v>153</v>
-      </c>
-      <c r="C238" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D238" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E238" s="42" t="s">
-        <v>154</v>
       </c>
       <c r="F238" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2937,18 +2936,18 @@
     <row r="239" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="43"/>
       <c r="B239" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C239" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D239" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E239" s="42" t="s">
         <v>155</v>
-      </c>
-      <c r="C239" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D239" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E239" s="42" t="s">
-        <v>156</v>
       </c>
       <c r="F239" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2962,18 +2961,18 @@
     <row r="240" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="43"/>
       <c r="B240" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="C240" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D240" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E240" s="42" t="s">
         <v>157</v>
-      </c>
-      <c r="C240" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D240" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E240" s="42" t="s">
-        <v>158</v>
       </c>
       <c r="F240" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2987,18 +2986,18 @@
     <row r="241" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="43"/>
       <c r="B241" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="C241" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D241" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E241" s="42" t="s">
         <v>159</v>
-      </c>
-      <c r="C241" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D241" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E241" s="42" t="s">
-        <v>160</v>
       </c>
       <c r="F241" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3011,18 +3010,18 @@
     </row>
     <row r="242" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B242" s="42" t="s">
+        <v>160</v>
+      </c>
+      <c r="C242" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D242" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E242" s="42" t="s">
         <v>161</v>
-      </c>
-      <c r="C242" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D242" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E242" s="42" t="s">
-        <v>162</v>
       </c>
       <c r="F242" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3035,18 +3034,18 @@
     </row>
     <row r="243" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B243" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="C243" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D243" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E243" s="42" t="s">
         <v>163</v>
-      </c>
-      <c r="C243" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D243" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E243" s="42" t="s">
-        <v>164</v>
       </c>
       <c r="F243" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3059,18 +3058,18 @@
     </row>
     <row r="244" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B244" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="C244" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D244" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E244" s="42" t="s">
         <v>165</v>
-      </c>
-      <c r="C244" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D244" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E244" s="42" t="s">
-        <v>166</v>
       </c>
       <c r="F244" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3083,21 +3082,21 @@
     </row>
     <row r="245" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="B245" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="B245" s="42" t="s">
+      <c r="C245" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D245" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E245" s="42" t="s">
         <v>168</v>
-      </c>
-      <c r="C245" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D245" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E245" s="42" t="s">
-        <v>169</v>
       </c>
       <c r="F245" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3111,45 +3110,45 @@
     <row r="246" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="44"/>
       <c r="B246" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="C246" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D246" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E246" s="42" t="s">
         <v>170</v>
       </c>
-      <c r="C246" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D246" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E246" s="42" t="s">
+      <c r="F246" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G246" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H246" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="F246" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G246" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H246" s="2" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B247" s="42" t="s">
+        <v>172</v>
+      </c>
+      <c r="C247" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D247" s="23" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E247" s="42" t="s">
         <v>173</v>
-      </c>
-      <c r="C247" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D247" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E247" s="42" t="s">
-        <v>174</v>
       </c>
       <c r="F247" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3188,7 +3187,7 @@
     <row r="273" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="274" s="18" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B274" s="16"/>
       <c r="C274" s="17"/>
@@ -3203,7 +3202,7 @@
         <v>58</v>
       </c>
       <c r="B275" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C275" s="28" t="n">
         <v>1</v>
@@ -3211,38 +3210,38 @@
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B276" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C276" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H276" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B276" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="C276" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H276" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B277" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C277" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H277" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="B277" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="C277" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H277" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B278" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C278" s="28" t="n">
         <v>1</v>
@@ -3256,7 +3255,7 @@
     <row r="288" customFormat="false" ht="0.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="298" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B298" s="16"/>
       <c r="C298" s="17"/>
@@ -3268,7 +3267,7 @@
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C299" s="38" t="s">
         <v>14</v>
@@ -3281,7 +3280,7 @@
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B300" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C300" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3290,7 +3289,7 @@
     </row>
     <row r="301" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B301" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C301" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3299,7 +3298,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B302" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C302" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3308,7 +3307,7 @@
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B303" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C303" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3327,7 +3326,7 @@
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C305" s="38" t="s">
         <v>14</v>
@@ -3338,14 +3337,14 @@
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B306" s="46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C306" s="45" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E306" s="46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F306" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3354,14 +3353,14 @@
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B307" s="46" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C307" s="45" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E307" s="46" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F307" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3370,14 +3369,14 @@
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B308" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="C308" s="45" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E308" s="46" t="s">
         <v>191</v>
-      </c>
-      <c r="C308" s="45" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E308" s="46" t="s">
-        <v>192</v>
       </c>
       <c r="F308" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3386,14 +3385,14 @@
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B309" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="C309" s="45" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E309" s="46" t="s">
         <v>193</v>
-      </c>
-      <c r="C309" s="45" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E309" s="46" t="s">
-        <v>194</v>
       </c>
       <c r="F309" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3402,14 +3401,14 @@
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B310" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="C310" s="45" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E310" s="46" t="s">
         <v>195</v>
-      </c>
-      <c r="C310" s="45" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E310" s="46" t="s">
-        <v>196</v>
       </c>
       <c r="F310" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3418,14 +3417,14 @@
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B311" s="46" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C311" s="45" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E311" s="46" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F311" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3434,14 +3433,14 @@
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B312" s="46" t="s">
+        <v>197</v>
+      </c>
+      <c r="C312" s="45" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E312" s="46" t="s">
         <v>198</v>
-      </c>
-      <c r="C312" s="45" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E312" s="46" t="s">
-        <v>199</v>
       </c>
       <c r="F312" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3450,14 +3449,14 @@
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B313" s="46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C313" s="45" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E313" s="46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F313" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3466,14 +3465,14 @@
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B314" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="C314" s="45" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E314" s="46" t="s">
         <v>201</v>
-      </c>
-      <c r="C314" s="45" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E314" s="46" t="s">
-        <v>202</v>
       </c>
       <c r="F314" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3482,14 +3481,14 @@
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B315" s="46" t="s">
+        <v>202</v>
+      </c>
+      <c r="C315" s="45" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E315" s="46" t="s">
         <v>203</v>
-      </c>
-      <c r="C315" s="45" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E315" s="46" t="s">
-        <v>204</v>
       </c>
       <c r="F315" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3498,14 +3497,14 @@
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B316" s="46" t="s">
+        <v>204</v>
+      </c>
+      <c r="C316" s="45" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E316" s="46" t="s">
         <v>205</v>
-      </c>
-      <c r="C316" s="45" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E316" s="46" t="s">
-        <v>206</v>
       </c>
       <c r="F316" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3514,14 +3513,14 @@
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B317" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="C317" s="45" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E317" s="46" t="s">
         <v>207</v>
-      </c>
-      <c r="C317" s="45" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E317" s="46" t="s">
-        <v>208</v>
       </c>
       <c r="F317" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3530,14 +3529,14 @@
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B318" s="46" t="s">
+        <v>208</v>
+      </c>
+      <c r="C318" s="45" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E318" s="46" t="s">
         <v>209</v>
-      </c>
-      <c r="C318" s="45" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E318" s="46" t="s">
-        <v>210</v>
       </c>
       <c r="F318" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3546,14 +3545,14 @@
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B319" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="C319" s="45" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E319" s="46" t="s">
         <v>211</v>
-      </c>
-      <c r="C319" s="45" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E319" s="46" t="s">
-        <v>212</v>
       </c>
       <c r="F319" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3562,14 +3561,14 @@
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B320" s="46" t="s">
+        <v>212</v>
+      </c>
+      <c r="C320" s="45" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E320" s="46" t="s">
         <v>213</v>
-      </c>
-      <c r="C320" s="45" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E320" s="46" t="s">
-        <v>214</v>
       </c>
       <c r="F320" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3578,14 +3577,14 @@
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B321" s="46" t="s">
+        <v>214</v>
+      </c>
+      <c r="C321" s="45" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E321" s="46" t="s">
         <v>215</v>
-      </c>
-      <c r="C321" s="45" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E321" s="46" t="s">
-        <v>216</v>
       </c>
       <c r="F321" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3594,16 +3593,16 @@
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E322" s="46" t="s">
-        <v>217</v>
-      </c>
-      <c r="F322" s="45" t="b">
+        <v>216</v>
+      </c>
+      <c r="F322" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3869,77 +3868,77 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.71"/>
   </cols>
   <sheetData>
-    <row r="1" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+    <row r="1" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="E1" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>221</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="47" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>222</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>223</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>224</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="b">
+      <c r="A3" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>228</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>231</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>232</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>46</v>
@@ -3947,7 +3946,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>37</v>
+        <v>232</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>233</v>
@@ -3958,7 +3957,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>235</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -3985,964 +3984,964 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="47" t="s">
+    <row r="1" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="48" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="48" t="s">
         <v>236</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="D1" s="48" t="s">
         <v>237</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="E1" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="F1" s="48" t="s">
         <v>239</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="G1" s="48" t="s">
         <v>240</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="H1" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="I1" s="48" t="s">
         <v>242</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="J1" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="K1" s="48" t="s">
         <v>244</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="L1" s="48" t="s">
         <v>245</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="M1" s="48" t="s">
         <v>246</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="N1" s="48" t="s">
         <v>247</v>
       </c>
-      <c r="N1" s="47" t="s">
+      <c r="O1" s="48" t="s">
         <v>248</v>
       </c>
-      <c r="O1" s="47" t="s">
-        <v>249</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="48" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="B2" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C2" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="47" t="s">
+      <c r="B3" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="48" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="48" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="48" t="s">
+        <v>194</v>
+      </c>
+      <c r="B6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C3" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="47" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="47" t="s">
-        <v>193</v>
-      </c>
-      <c r="B5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="47" t="s">
-        <v>195</v>
-      </c>
-      <c r="B6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="47" t="s">
+      <c r="B7" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="B8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="48" t="s">
         <v>186</v>
       </c>
-      <c r="B7" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C7" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="47" t="s">
-        <v>198</v>
-      </c>
-      <c r="B8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="B9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="49" t="b">
+      <c r="B9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="B10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O10" s="49" t="b">
+      <c r="A10" s="48" t="s">
+        <v>200</v>
+      </c>
+      <c r="B10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="B11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O11" s="49" t="b">
+      <c r="A11" s="48" t="s">
+        <v>202</v>
+      </c>
+      <c r="B11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="47" t="s">
-        <v>205</v>
-      </c>
-      <c r="B12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O12" s="49" t="b">
+      <c r="A12" s="48" t="s">
+        <v>204</v>
+      </c>
+      <c r="B12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O12" s="50" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="47" t="s">
-        <v>207</v>
-      </c>
-      <c r="B13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O13" s="49" t="b">
+      <c r="A13" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O13" s="50" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="47" t="s">
-        <v>209</v>
-      </c>
-      <c r="B14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O14" s="49" t="b">
+      <c r="A14" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="B14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O14" s="50" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="47" t="s">
-        <v>211</v>
-      </c>
-      <c r="B15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O15" s="49" t="b">
+      <c r="A15" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="B15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="47" t="s">
-        <v>213</v>
-      </c>
-      <c r="B16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O16" s="49" t="b">
+      <c r="A16" s="48" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Ordering the Processing scripts, cleaning those unnecesary scripts, some scripts need to been completed, next stept complete them
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigBE1.xlsx
+++ b/ConfigFiles/ConfigBE1.xlsx
@@ -57,7 +57,7 @@
     <t xml:space="preserve">Relative Path</t>
   </si>
   <si>
-    <t xml:space="preserve">Simulations/simulationBE_No_Clustering_No_Reservoir_Level</t>
+    <t xml:space="preserve">Simulations/simulationBE_Standard</t>
   </si>
   <si>
     <t xml:space="preserve">This section defines the output of the pre-processing (which is the input of the DispaSet solver)</t>
@@ -135,598 +135,598 @@
     <t xml:space="preserve">List</t>
   </si>
   <si>
+    <t xml:space="preserve">Standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This sections defines parameters that influence the formulation of the problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserve calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These parameters influence both the pre-processing (e.g. in LP clustering, all units are aggregated by type)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allow Curtailment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">and the solver (some constraints are removed when solving in LP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro Scheduling Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro scheduling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These parameters influence how HDAM and HPHS units are operated (e.g. if Standard: scaled reservoir levels are computed internally</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydro scheduling horizon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These parameters influence the horizon of the hydro scheduling (e.g. if Annual: reservoirs are computed for the whole year, if Stop-date driven: computation of reservoirs is driven by the start and stop date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial/Final resevoir levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-&gt; Initial level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This value imposes the inital (relative) reservoir levels if the option is set to true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;- Final level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This value imposes the final (relative) reservoir levels if the option is set to true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/Load_RealTime/##/1h/2023.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flexible Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/OutageFactors/##/1h/2023.csv </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This section provides the paths to the raw data used to generate the Dispa-SET simulation template. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power plant data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/PowerPlants/##/2023.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The path is an absolute path or a relative path to this config file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renewables AF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/AvailabilityFactors/##/1h/2023.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Shedding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For datasets which have one file per country, replace the country code (2 characters) in the path by ##. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/NTC/1h/2023.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for example: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical flows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/CrossBorderFlows/1h/2023.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../data/Demand/##/2014/load.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scaled inflows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/HydroData/ScaledInflows/##/1h/2023.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">will fetch one load.csv file per country, by replacing ## with FR, DE, NL, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reservoir Levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperatures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geo Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2 Demand (P2H2 - rigid)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2 Demand (P2Liquid - flexible)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2 Capacities (P2Liquid - flexible)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserves Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserves Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Demand flexibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of equivalent storage hours for the flexibile demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of quick start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of the 2U reserve that can be covered by quick start units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of CO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: https://dev-rad-carbon-pricing.pantheonsite.io/about#download-data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Unserved Heat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Shedding Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The least amount that customers are willing to recieve to reduce the electricity demand. EUR/MWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Transmission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price related to the usage of tranmission lines (in €/MWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Unserved H2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curtailment Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Nuclear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Black coal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/FuelPrices/Coal/2015.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Gas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/FuelPrices/Gas/2015.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All fuel prices are in EUR/MWh of primary energy (lower heating value)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Fuel-Oil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/FuelPrices/Oil/2015.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ahdb.org.uk/fuel-prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database/FuelPrices/Biomass/2015.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Lignite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Peat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Ammonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of Lost Load (VOLL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of lost load  in EUR/MWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Price of Spillage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost occurring due to involuntary water spillage in hydro resrvoirs EUR/MWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value of water (for unsatisfied water reservoir levels) EUR/MWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Active zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Countries to consider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUTS1 codes (ISO 3166-1 standard) of the simulated countries.                                      NB: all the selected countries must be present in the data files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZZ3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NB: Ireland (IE) includes Northern Ireland. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NB: UK is not considered as zone but GB is.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input modifiers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mult. Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The input modifies can be used to quickly modify the data from the database. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The specified factor scales up or down the capacity and the generation of the specified technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserve Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participation to reserve markets (CHP units)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participation to reserve markets (Non-CHP units)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2HT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HPHS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HYHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WSHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REHE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALKE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WTOF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOXE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BATS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEVS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2GS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End of the Config file. This must be line number 325!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulation Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resrve calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacity Correction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ignore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display Warning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zonal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stop-date driven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LP clustered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Probabilistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add plants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer clustering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exogenous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scale-up capacities</t>
+  </si>
+  <si>
     <t xml:space="preserve">No clustering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This sections defines parameters that influence the formulation of the problem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reserve calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">These parameters influence both the pre-processing (e.g. in LP clustering, all units are aggregated by type)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allow Curtailment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">and the solver (some constraints are removed when solving in LP)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hydro Scheduling Options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hydro scheduling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">These parameters influence how HDAM and HPHS units are operated (e.g. if Standard: scaled reservoir levels are computed internally</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hydro scheduling horizon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Annual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">These parameters influence the horizon of the hydro scheduling (e.g. if Annual: reservoirs are computed for the whole year, if Stop-date driven: computation of reservoirs is driven by the start and stop date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initial/Final resevoir levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-&gt; Initial level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Default value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This value imposes the inital (relative) reservoir levels if the option is set to true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;- Final level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This value imposes the final (relative) reservoir levels if the option is set to true</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/Load_RealTime/##/1h/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flexible Demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/OutageFactors/##/1h/2023.csv </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This section provides the paths to the raw data used to generate the Dispa-SET simulation template. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Power plant data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/PowerPlants/##/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The path is an absolute path or a relative path to this config file</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renewables AF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/AvailabilityFactors/##/1h/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load Shedding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For datasets which have one file per country, replace the country code (2 characters) in the path by ##. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NTC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/NTC/1h/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">for example: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Historical flows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/CrossBorderFlows/1h/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">../data/Demand/##/2014/load.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scaled inflows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/HydroData/ScaledInflows/##/1h/2023.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">will fetch one load.csv file per country, by replacing ## with FR, DE, NL, etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reservoir Levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heat Demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperatures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geo Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2 Demand (P2H2 - rigid)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2 Demand (P2Liquid - flexible)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2 Capacities (P2Liquid - flexible)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reserves Up</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reserves Down</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demand flexibility</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of equivalent storage hours for the flexibile demand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share of quick start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share of the 2U reserve that can be covered by quick start units</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of CO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source: https://dev-rad-carbon-pricing.pantheonsite.io/about#download-data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Unserved Heat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Load Shedding Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The least amount that customers are willing to recieve to reduce the electricity demand. EUR/MWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Transmission</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price related to the usage of tranmission lines (in €/MWh)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Unserved H2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Curtailment Cost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Nuclear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Black coal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/FuelPrices/Coal/2015.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Gas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/FuelPrices/Gas/2015.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All fuel prices are in EUR/MWh of primary energy (lower heating value)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Fuel-Oil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/FuelPrices/Oil/2015.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://ahdb.org.uk/fuel-prices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/FuelPrices/Biomass/2015.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Lignite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Peat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Ammonia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value of Lost Load (VOLL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value of lost load  in EUR/MWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Price of Spillage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost occurring due to involuntary water spillage in hydro resrvoirs EUR/MWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value of water (for unsatisfied water reservoir levels) EUR/MWh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone Options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Active zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Countries to consider</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUTS1 codes (ISO 3166-1 standard) of the simulated countries.                                      NB: all the selected countries must be present in the data files</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZZ3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NB: Ireland (IE) includes Northern Ireland. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NB: UK is not considered as zone but GB is.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Input modifiers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mult. Factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The input modifies can be used to quickly modify the data from the database. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Solar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The specified factor scales up or down the capacity and the generation of the specified technology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Storage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reserve Options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participation to reserve markets (CHP units)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COMC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ICEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Participation to reserve markets (Non-CHP units)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2HT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HDAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HROR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HPHS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HYHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WSHP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHOT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REHE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALKE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WTOF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WTON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOXE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BATS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DMFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BEVS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P2GS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCSP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">End of the Config file. This must be line number 325!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simulation Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resrve calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacity Correction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ignore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Display Warning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zonal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stop-date driven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LP clustered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Probabilistic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add plants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integer clustering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exogenous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scale-up capacities</t>
   </si>
   <si>
     <t xml:space="preserve">BIO</t>
@@ -953,7 +953,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1140,10 +1140,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1337,8 +1333,8 @@
   </sheetPr>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C134" activeCellId="0" sqref="C134"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3595,7 +3591,7 @@
       <c r="E322" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="F322" s="47" t="b">
+      <c r="F322" s="45" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3868,77 +3864,77 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.71"/>
   </cols>
   <sheetData>
-    <row r="1" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="48" t="s">
+    <row r="1" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>218</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="47" t="s">
         <v>220</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="47" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49" t="b">
+      <c r="A2" s="48" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>221</v>
+        <v>37</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>222</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>223</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="49" t="b">
+      <c r="A3" s="48" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>227</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>230</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>231</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>46</v>
@@ -3946,18 +3942,18 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>233</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3984,964 +3980,964 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="48" t="s">
+    <row r="1" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="47" t="s">
         <v>235</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="47" t="s">
         <v>237</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="47" t="s">
         <v>238</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="47" t="s">
         <v>239</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="47" t="s">
         <v>240</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="47" t="s">
         <v>241</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="47" t="s">
         <v>242</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="47" t="s">
         <v>244</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="47" t="s">
         <v>245</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="M1" s="47" t="s">
         <v>246</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="N1" s="47" t="s">
         <v>247</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="47" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C2" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D2" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="50" t="b">
+      <c r="B2" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C3" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J3" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M3" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="50" t="b">
+      <c r="B3" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>190</v>
       </c>
-      <c r="B4" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M4" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="50" t="b">
+      <c r="B4" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>192</v>
       </c>
-      <c r="B5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="50" t="b">
+      <c r="B5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>194</v>
       </c>
-      <c r="B6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N6" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O6" s="50" t="b">
+      <c r="B6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N6" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O6" s="49" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C7" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J7" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="50" t="b">
+      <c r="B7" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="47" t="s">
         <v>197</v>
       </c>
-      <c r="B8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="50" t="b">
+      <c r="B8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D9" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="50" t="b">
+      <c r="B9" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="47" t="s">
         <v>200</v>
       </c>
-      <c r="B10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O10" s="50" t="b">
+      <c r="B10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="47" t="s">
         <v>202</v>
       </c>
-      <c r="B11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O11" s="50" t="b">
+      <c r="B11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="47" t="s">
         <v>204</v>
       </c>
-      <c r="B12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N12" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O12" s="50" t="b">
+      <c r="B12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N12" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O12" s="49" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="47" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N13" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O13" s="50" t="b">
+      <c r="B13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O13" s="49" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="47" t="s">
         <v>208</v>
       </c>
-      <c r="B14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N14" s="50" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O14" s="50" t="b">
+      <c r="B14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="49" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O14" s="49" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="48" t="s">
+      <c r="A15" s="47" t="s">
         <v>210</v>
       </c>
-      <c r="B15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O15" s="50" t="b">
+      <c r="B15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="47" t="s">
         <v>212</v>
       </c>
-      <c r="B16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="50" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O16" s="50" t="b">
+      <c r="B16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="49" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
changes in the total capacity per production type downloading script
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigBE1.xlsx
+++ b/ConfigFiles/ConfigBE1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="245">
   <si>
     <t xml:space="preserve">Dispa-SET Configuration File (v20.02)</t>
   </si>
@@ -57,7 +57,7 @@
     <t xml:space="preserve">Relative Path</t>
   </si>
   <si>
-    <t xml:space="preserve">Simulations/simulationBE_NoClustering</t>
+    <t xml:space="preserve">Simulations/simulationBE_DE_FR_NoClustering</t>
   </si>
   <si>
     <t xml:space="preserve">This section defines the output of the pre-processing (which is the input of the DispaSet solver)</t>
@@ -210,7 +210,7 @@
     <t xml:space="preserve">Outages</t>
   </si>
   <si>
-    <t xml:space="preserve">Database/OutageFactors/##/1h/2023.csv </t>
+    <t xml:space="preserve">Database/OutageFactors/##/1h/2023.csv</t>
   </si>
   <si>
     <t xml:space="preserve">This section provides the paths to the raw data used to generate the Dispa-SET simulation template. </t>
@@ -339,31 +339,19 @@
     <t xml:space="preserve">Price of Black coal</t>
   </si>
   <si>
-    <t xml:space="preserve">Database/FuelPrices/Coal/2015.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">Price of Gas</t>
   </si>
   <si>
-    <t xml:space="preserve">Database/FuelPrices/Gas/2015.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">All fuel prices are in EUR/MWh of primary energy (lower heating value)</t>
   </si>
   <si>
     <t xml:space="preserve">Price of Fuel-Oil</t>
   </si>
   <si>
-    <t xml:space="preserve">Database/FuelPrices/Oil/2015.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ahdb.org.uk/fuel-prices</t>
   </si>
   <si>
     <t xml:space="preserve">Price of Biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database/FuelPrices/Biomass/2015.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Price of Lignite</t>
@@ -953,7 +941,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1140,6 +1128,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1333,7 +1325,7 @@
   </sheetPr>
   <dimension ref="A1:H330"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -1537,7 +1529,7 @@
       <c r="G33" s="16"/>
       <c r="H33" s="16"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -2367,9 +2359,7 @@
       <c r="B182" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C182" s="32" t="s">
-        <v>105</v>
-      </c>
+      <c r="C182" s="32"/>
       <c r="D182" s="25" t="s">
         <v>20</v>
       </c>
@@ -2382,14 +2372,12 @@
     </row>
     <row r="183" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B183" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C183" s="32" t="s">
-        <v>107</v>
-      </c>
+      <c r="C183" s="32"/>
       <c r="D183" s="25" t="s">
         <v>20</v>
       </c>
@@ -2400,19 +2388,17 @@
         <v>44</v>
       </c>
       <c r="H183" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B184" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C184" s="32" t="s">
-        <v>110</v>
-      </c>
+      <c r="C184" s="32"/>
       <c r="D184" s="25" t="s">
         <v>20</v>
       </c>
@@ -2423,19 +2409,17 @@
         <v>61</v>
       </c>
       <c r="H184" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B185" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C185" s="32" t="s">
-        <v>113</v>
-      </c>
+      <c r="C185" s="32"/>
       <c r="D185" s="25" t="s">
         <v>20</v>
       </c>
@@ -2448,7 +2432,7 @@
     </row>
     <row r="186" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B186" s="19" t="s">
         <v>10</v>
@@ -2466,7 +2450,7 @@
     </row>
     <row r="187" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B187" s="19" t="s">
         <v>10</v>
@@ -2484,7 +2468,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B188" s="19" t="s">
         <v>10</v>
@@ -2517,7 +2501,7 @@
     <row r="204" customFormat="false" ht="13.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="205" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E205" s="21" t="s">
         <v>53</v>
@@ -2526,12 +2510,12 @@
         <v>100000</v>
       </c>
       <c r="H205" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="206" s="2" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E206" s="21" t="s">
         <v>53</v>
@@ -2540,12 +2524,12 @@
         <v>401</v>
       </c>
       <c r="H206" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="207" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E207" s="21" t="s">
         <v>53</v>
@@ -2554,7 +2538,7 @@
         <v>400</v>
       </c>
       <c r="H207" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.5" hidden="true" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2578,34 +2562,34 @@
     </row>
     <row r="225" s="41" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A225" s="12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B225" s="38" t="s">
         <v>14</v>
       </c>
       <c r="C225" s="12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D225" s="39" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E225" s="38" t="s">
         <v>14</v>
       </c>
       <c r="F225" s="12" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G225" s="12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H225" s="40"/>
     </row>
     <row r="226" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B226" s="42" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C226" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2616,7 +2600,7 @@
         <v>0</v>
       </c>
       <c r="E226" s="42" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F226" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2629,10 +2613,10 @@
     </row>
     <row r="227" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A227" s="43" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B227" s="42" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C227" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2643,7 +2627,7 @@
         <v>0</v>
       </c>
       <c r="E227" s="42" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F227" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2657,7 +2641,7 @@
     <row r="228" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A228" s="43"/>
       <c r="B228" s="42" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C228" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2668,7 +2652,7 @@
         <v>0</v>
       </c>
       <c r="E228" s="42" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F228" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2682,7 +2666,7 @@
     <row r="229" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A229" s="43"/>
       <c r="B229" s="42" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C229" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2693,7 +2677,7 @@
         <v>0</v>
       </c>
       <c r="E229" s="42" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F229" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2707,7 +2691,7 @@
     <row r="230" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A230" s="43"/>
       <c r="B230" s="42" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C230" s="23" t="b">
         <f aca="false">TRUE()</f>
@@ -2718,7 +2702,7 @@
         <v>0</v>
       </c>
       <c r="E230" s="42" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F230" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2732,7 +2716,7 @@
     <row r="231" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A231" s="43"/>
       <c r="B231" s="42" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C231" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2743,7 +2727,7 @@
         <v>0</v>
       </c>
       <c r="E231" s="42" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F231" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2757,7 +2741,7 @@
     <row r="232" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A232" s="43"/>
       <c r="B232" s="42" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C232" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2768,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="E232" s="42" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F232" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2782,7 +2766,7 @@
     <row r="233" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A233" s="43"/>
       <c r="B233" s="42" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C233" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2793,7 +2777,7 @@
         <v>0</v>
       </c>
       <c r="E233" s="42" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F233" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2807,7 +2791,7 @@
     <row r="234" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A234" s="43"/>
       <c r="B234" s="42" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C234" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2818,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="E234" s="42" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F234" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2832,7 +2816,7 @@
     <row r="235" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A235" s="43"/>
       <c r="B235" s="42" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C235" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2843,7 +2827,7 @@
         <v>0</v>
       </c>
       <c r="E235" s="42" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F235" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2857,18 +2841,17 @@
     <row r="236" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A236" s="43"/>
       <c r="B236" s="42" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C236" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D236" s="23" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E236" s="42" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F236" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2882,7 +2865,7 @@
     <row r="237" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A237" s="43"/>
       <c r="B237" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C237" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2893,7 +2876,7 @@
         <v>0</v>
       </c>
       <c r="E237" s="42" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F237" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2907,7 +2890,7 @@
     <row r="238" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A238" s="43"/>
       <c r="B238" s="42" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C238" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2918,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="E238" s="42" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F238" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2932,7 +2915,7 @@
     <row r="239" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A239" s="43"/>
       <c r="B239" s="42" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C239" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2943,7 +2926,7 @@
         <v>0</v>
       </c>
       <c r="E239" s="42" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F239" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2957,7 +2940,7 @@
     <row r="240" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A240" s="43"/>
       <c r="B240" s="42" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C240" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2968,7 +2951,7 @@
         <v>0</v>
       </c>
       <c r="E240" s="42" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F240" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -2982,10 +2965,9 @@
     <row r="241" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A241" s="43"/>
       <c r="B241" s="42" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C241" s="23" t="b">
-        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D241" s="23" t="b">
@@ -2993,7 +2975,7 @@
         <v>0</v>
       </c>
       <c r="E241" s="42" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F241" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3006,18 +2988,17 @@
     </row>
     <row r="242" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B242" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C242" s="23" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D242" s="23" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E242" s="42" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F242" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3030,7 +3011,7 @@
     </row>
     <row r="243" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B243" s="42" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C243" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3041,7 +3022,7 @@
         <v>0</v>
       </c>
       <c r="E243" s="42" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F243" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3054,7 +3035,7 @@
     </row>
     <row r="244" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B244" s="42" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C244" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3065,7 +3046,7 @@
         <v>0</v>
       </c>
       <c r="E244" s="42" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F244" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3078,10 +3059,10 @@
     </row>
     <row r="245" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A245" s="44" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B245" s="42" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C245" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3092,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="E245" s="42" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F245" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3106,7 +3087,7 @@
     <row r="246" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A246" s="44"/>
       <c r="B246" s="42" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C246" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3117,7 +3098,7 @@
         <v>0</v>
       </c>
       <c r="E246" s="42" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F246" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3128,12 +3109,12 @@
         <v>0</v>
       </c>
       <c r="H246" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B247" s="42" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C247" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3144,7 +3125,7 @@
         <v>0</v>
       </c>
       <c r="E247" s="42" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F247" s="23" t="b">
         <f aca="false">FALSE()</f>
@@ -3183,7 +3164,7 @@
     <row r="273" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="274" s="18" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A274" s="15" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B274" s="16"/>
       <c r="C274" s="17"/>
@@ -3198,7 +3179,7 @@
         <v>58</v>
       </c>
       <c r="B275" s="21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C275" s="28" t="n">
         <v>1</v>
@@ -3206,38 +3187,38 @@
     </row>
     <row r="276" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B276" s="21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C276" s="28" t="n">
         <v>1</v>
       </c>
       <c r="H276" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B277" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C277" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H277" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C277" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H277" s="2" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B278" s="21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C278" s="28" t="n">
         <v>1</v>
@@ -3251,7 +3232,7 @@
     <row r="288" customFormat="false" ht="0.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="298" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="15" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B298" s="16"/>
       <c r="C298" s="17"/>
@@ -3263,7 +3244,7 @@
     </row>
     <row r="299" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C299" s="38" t="s">
         <v>14</v>
@@ -3276,7 +3257,7 @@
     </row>
     <row r="300" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B300" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C300" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3285,7 +3266,7 @@
     </row>
     <row r="301" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B301" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C301" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3294,7 +3275,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B302" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C302" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3303,7 +3284,7 @@
     </row>
     <row r="303" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B303" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C303" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3322,7 +3303,7 @@
     </row>
     <row r="305" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C305" s="38" t="s">
         <v>14</v>
@@ -3333,14 +3314,14 @@
     </row>
     <row r="306" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B306" s="46" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C306" s="45" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E306" s="46" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F306" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3349,14 +3330,14 @@
     </row>
     <row r="307" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B307" s="46" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C307" s="45" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E307" s="46" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F307" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3365,14 +3346,14 @@
     </row>
     <row r="308" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B308" s="46" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C308" s="45" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E308" s="46" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F308" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3381,14 +3362,14 @@
     </row>
     <row r="309" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B309" s="46" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C309" s="45" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E309" s="46" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F309" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3397,14 +3378,14 @@
     </row>
     <row r="310" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B310" s="46" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C310" s="45" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E310" s="46" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F310" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3413,14 +3394,14 @@
     </row>
     <row r="311" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B311" s="46" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C311" s="45" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E311" s="46" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F311" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3429,14 +3410,14 @@
     </row>
     <row r="312" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B312" s="46" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C312" s="45" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E312" s="46" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F312" s="45" t="b">
         <f aca="false">TRUE()</f>
@@ -3445,14 +3426,14 @@
     </row>
     <row r="313" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B313" s="46" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C313" s="45" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E313" s="46" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F313" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3461,14 +3442,14 @@
     </row>
     <row r="314" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B314" s="46" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C314" s="45" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E314" s="46" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F314" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3477,14 +3458,14 @@
     </row>
     <row r="315" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B315" s="46" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C315" s="45" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E315" s="46" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F315" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3493,14 +3474,14 @@
     </row>
     <row r="316" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B316" s="46" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C316" s="45" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E316" s="46" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F316" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3509,14 +3490,14 @@
     </row>
     <row r="317" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B317" s="46" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C317" s="45" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E317" s="46" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F317" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3525,14 +3506,14 @@
     </row>
     <row r="318" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B318" s="46" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C318" s="45" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="E318" s="46" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F318" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3541,14 +3522,14 @@
     </row>
     <row r="319" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B319" s="46" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C319" s="45" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E319" s="46" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F319" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3557,14 +3538,14 @@
     </row>
     <row r="320" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B320" s="46" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C320" s="45" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E320" s="46" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F320" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3573,14 +3554,14 @@
     </row>
     <row r="321" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B321" s="46" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C321" s="45" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E321" s="46" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F321" s="45" t="b">
         <f aca="false">FALSE()</f>
@@ -3589,16 +3570,16 @@
     </row>
     <row r="322" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E322" s="46" t="s">
-        <v>216</v>
-      </c>
-      <c r="F322" s="45" t="b">
+        <v>212</v>
+      </c>
+      <c r="F322" s="47" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3851,7 +3832,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -3864,39 +3845,39 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.71"/>
   </cols>
   <sheetData>
-    <row r="1" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47" t="s">
+    <row r="1" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="47" t="s">
-        <v>218</v>
+      <c r="B1" s="48" t="s">
+        <v>214</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D1" s="47" t="s">
-        <v>220</v>
-      </c>
-      <c r="E1" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="48" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="b">
+      <c r="A2" s="49" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>40</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>46</v>
@@ -3906,49 +3887,49 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="b">
+      <c r="A3" s="49" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>223</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>224</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>225</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>226</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3974,970 +3955,970 @@
   </sheetPr>
   <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="48" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="47" t="s">
+    <row r="1" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="48" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>234</v>
+      </c>
+      <c r="F1" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="G1" s="48" t="s">
         <v>236</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="H1" s="48" t="s">
         <v>237</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="I1" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="J1" s="48" t="s">
         <v>239</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="K1" s="48" t="s">
         <v>240</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="L1" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="M1" s="48" t="s">
         <v>242</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="N1" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="O1" s="48" t="s">
         <v>244</v>
       </c>
-      <c r="L1" s="47" t="s">
-        <v>245</v>
-      </c>
-      <c r="M1" s="47" t="s">
-        <v>246</v>
-      </c>
-      <c r="N1" s="47" t="s">
-        <v>247</v>
-      </c>
-      <c r="O1" s="47" t="s">
-        <v>248</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="47" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C2" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="49" t="b">
+      <c r="A2" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="47" t="s">
-        <v>184</v>
-      </c>
-      <c r="B3" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C3" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N3" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="49" t="b">
+      <c r="A3" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="48" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="48" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="B4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="47" t="s">
-        <v>192</v>
-      </c>
-      <c r="B5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="47" t="s">
-        <v>194</v>
-      </c>
-      <c r="B6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N6" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O6" s="49" t="b">
+      <c r="B6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N6" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O6" s="50" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="47" t="s">
-        <v>185</v>
-      </c>
-      <c r="B7" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C7" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N7" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="49" t="b">
+      <c r="A7" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O7" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="47" t="s">
-        <v>197</v>
-      </c>
-      <c r="B8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N8" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O8" s="49" t="b">
+      <c r="A8" s="48" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="B9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N9" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O9" s="49" t="b">
+      <c r="A9" s="48" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="48" t="s">
+        <v>198</v>
+      </c>
+      <c r="B11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O11" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="48" t="s">
         <v>200</v>
       </c>
-      <c r="B10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O10" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="47" t="s">
+      <c r="B12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O12" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="48" t="s">
         <v>202</v>
       </c>
-      <c r="B11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O11" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="47" t="s">
+      <c r="B13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O13" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="B12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O12" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="47" t="s">
+      <c r="B14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="K14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="M14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O14" s="50" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O13" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="47" t="s">
+      <c r="B15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="B14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="C14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="E14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="J14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="K14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="L14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="M14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="N14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="O14" s="49" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="47" t="s">
-        <v>210</v>
-      </c>
-      <c r="B15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O15" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="47" t="s">
-        <v>212</v>
-      </c>
-      <c r="B16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="F16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="L16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="M16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="N16" s="49" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="O16" s="49" t="b">
+      <c r="B16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="50" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="50" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>